<commit_message>
MainMenu & Admin menu
</commit_message>
<xml_diff>
--- a/DataStorage/TotalHistory.xlsx
+++ b/DataStorage/TotalHistory.xlsx
@@ -7,15 +7,14 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="user5585413083" sheetId="1" r:id="rId1"/>
-    <sheet name="user243378934" sheetId="2" r:id="rId2"/>
+    <sheet name="user243378934" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="63">
   <si>
     <t>Дата</t>
   </si>
@@ -32,10 +31,10 @@
     <t>Описание</t>
   </si>
   <si>
-    <t>31.10.2022</t>
-  </si>
-  <si>
-    <t>03:31:54</t>
+    <t>03.11.2022</t>
+  </si>
+  <si>
+    <t>19:48:39</t>
   </si>
   <si>
     <t>Старт</t>
@@ -44,88 +43,166 @@
     <t>Начало сохранения истории пользователя</t>
   </si>
   <si>
-    <t>03:27:21</t>
-  </si>
-  <si>
-    <t>03:34:08</t>
-  </si>
-  <si>
-    <t>03:34:23</t>
-  </si>
-  <si>
-    <t>03:34:34</t>
-  </si>
-  <si>
-    <t>04:38:13</t>
-  </si>
-  <si>
-    <t>04:38:19</t>
-  </si>
-  <si>
-    <t>04:40:54</t>
-  </si>
-  <si>
-    <t>04:43:12</t>
-  </si>
-  <si>
-    <t>04:43:44</t>
-  </si>
-  <si>
-    <t>04:51:41</t>
-  </si>
-  <si>
-    <t>04:52:08</t>
-  </si>
-  <si>
-    <t>04:53:30</t>
-  </si>
-  <si>
-    <t>04:54:05</t>
-  </si>
-  <si>
-    <t>05:49:43</t>
-  </si>
-  <si>
-    <t>sendMessage</t>
+    <t>Начал смотреть онбординг</t>
+  </si>
+  <si>
+    <t>19:49:09</t>
   </si>
   <si>
     <t>Отправил сообщение</t>
   </si>
   <si>
-    <t>05:50:37</t>
-  </si>
-  <si>
-    <t>05:51:17</t>
-  </si>
-  <si>
-    <t>05:51:44</t>
-  </si>
-  <si>
-    <t>05:52:04</t>
-  </si>
-  <si>
-    <t>05:53:08</t>
-  </si>
-  <si>
-    <t>05:59:47</t>
-  </si>
-  <si>
-    <t>06:03:32</t>
-  </si>
-  <si>
-    <t>06:05:17</t>
-  </si>
-  <si>
-    <t>06:12:02</t>
-  </si>
-  <si>
-    <t>06:18:29</t>
-  </si>
-  <si>
-    <t>06:18:50</t>
-  </si>
-  <si>
-    <t>06:20:04</t>
+    <t>Далее</t>
+  </si>
+  <si>
+    <t>19:50:21</t>
+  </si>
+  <si>
+    <t>Админ</t>
+  </si>
+  <si>
+    <t>19:50:24</t>
+  </si>
+  <si>
+    <t>kek</t>
+  </si>
+  <si>
+    <t>19:50:43</t>
+  </si>
+  <si>
+    <t>Понятно. Начнем!</t>
+  </si>
+  <si>
+    <t>20:19:26</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>20:20:31</t>
+  </si>
+  <si>
+    <t>20:20:35</t>
+  </si>
+  <si>
+    <t>20:20:39</t>
+  </si>
+  <si>
+    <t>Unknown</t>
+  </si>
+  <si>
+    <t>20:21:34</t>
+  </si>
+  <si>
+    <t>20:21:49</t>
+  </si>
+  <si>
+    <t>20:23:30</t>
+  </si>
+  <si>
+    <t>20:26:11</t>
+  </si>
+  <si>
+    <t>20:27:14</t>
+  </si>
+  <si>
+    <t>20:28:26</t>
+  </si>
+  <si>
+    <t>20:29:33</t>
+  </si>
+  <si>
+    <t>20:29:48</t>
+  </si>
+  <si>
+    <t>Выгрузить данные</t>
+  </si>
+  <si>
+    <t>20:29:51</t>
+  </si>
+  <si>
+    <t>Стянуть новые тексты из гугл таблицы</t>
+  </si>
+  <si>
+    <t>20:34:40</t>
+  </si>
+  <si>
+    <t>Emergency reboot</t>
+  </si>
+  <si>
+    <t>20:34:57</t>
+  </si>
+  <si>
+    <t>20:35:46</t>
+  </si>
+  <si>
+    <t>20:36:16</t>
+  </si>
+  <si>
+    <t>20:36:18</t>
+  </si>
+  <si>
+    <t>20:36:21</t>
+  </si>
+  <si>
+    <t>Я не хочу делать упражнения, просто хочу переключиться</t>
+  </si>
+  <si>
+    <t>20:36:24</t>
+  </si>
+  <si>
+    <t>20:36:29</t>
+  </si>
+  <si>
+    <t>20:36:44</t>
+  </si>
+  <si>
+    <t>Перейти к упражнениям</t>
+  </si>
+  <si>
+    <t>20:36:54</t>
+  </si>
+  <si>
+    <t>20:36:57</t>
+  </si>
+  <si>
+    <t>20:37:50</t>
+  </si>
+  <si>
+    <t>20:37:52</t>
+  </si>
+  <si>
+    <t>20:37:53</t>
+  </si>
+  <si>
+    <t>20:37:55</t>
+  </si>
+  <si>
+    <t>20:39:39</t>
+  </si>
+  <si>
+    <t>20:39:40</t>
+  </si>
+  <si>
+    <t>20:39:41</t>
+  </si>
+  <si>
+    <t>20:39:42</t>
+  </si>
+  <si>
+    <t>20:41:43</t>
+  </si>
+  <si>
+    <t>20:42:32</t>
+  </si>
+  <si>
+    <t>Главное меню</t>
+  </si>
+  <si>
+    <t>20:42:35</t>
+  </si>
+  <si>
+    <t>20:42:38</t>
   </si>
 </sst>
 </file>
@@ -466,7 +543,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E64"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -513,75 +590,18 @@
         <v>8</v>
       </c>
     </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E27"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="4.7109375" customWidth="1"/>
-    <col min="2" max="2" width="5.7109375" customWidth="1"/>
-    <col min="3" max="3" width="6.7109375" customWidth="1"/>
-    <col min="4" max="4" width="7.7109375" customWidth="1"/>
-    <col min="5" max="5" width="50.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2">
-        <v>44</v>
-      </c>
-      <c r="D2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" t="s">
-        <v>8</v>
-      </c>
-    </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C3">
         <v>44</v>
       </c>
       <c r="D3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -589,16 +609,16 @@
         <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C4">
         <v>44</v>
       </c>
       <c r="D4" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E4" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -606,16 +626,16 @@
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C5">
         <v>44</v>
       </c>
       <c r="D5" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E5" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -623,16 +643,16 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C6">
         <v>44</v>
       </c>
       <c r="D6" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E6" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -640,16 +660,16 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C7">
         <v>44</v>
       </c>
       <c r="D7" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E7" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -657,16 +677,13 @@
         <v>5</v>
       </c>
       <c r="B8" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C8">
         <v>44</v>
       </c>
       <c r="D8" t="s">
-        <v>7</v>
-      </c>
-      <c r="E8" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -674,16 +691,16 @@
         <v>5</v>
       </c>
       <c r="B9" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C9">
         <v>44</v>
       </c>
       <c r="D9" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E9" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -691,16 +708,16 @@
         <v>5</v>
       </c>
       <c r="B10" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C10">
         <v>44</v>
       </c>
       <c r="D10" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E10" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -708,16 +725,16 @@
         <v>5</v>
       </c>
       <c r="B11" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="C11">
         <v>44</v>
       </c>
       <c r="D11" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E11" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -725,16 +742,13 @@
         <v>5</v>
       </c>
       <c r="B12" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C12">
         <v>44</v>
       </c>
       <c r="D12" t="s">
-        <v>7</v>
-      </c>
-      <c r="E12" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -742,16 +756,16 @@
         <v>5</v>
       </c>
       <c r="B13" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="C13">
         <v>44</v>
       </c>
       <c r="D13" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E13" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -759,16 +773,16 @@
         <v>5</v>
       </c>
       <c r="B14" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="C14">
         <v>44</v>
       </c>
       <c r="D14" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E14" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -776,13 +790,13 @@
         <v>5</v>
       </c>
       <c r="B15" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="C15">
         <v>44</v>
       </c>
       <c r="D15" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="E15" t="s">
         <v>24</v>
@@ -793,13 +807,13 @@
         <v>5</v>
       </c>
       <c r="B16" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C16">
         <v>44</v>
       </c>
       <c r="D16" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="E16" t="s">
         <v>24</v>
@@ -810,16 +824,13 @@
         <v>5</v>
       </c>
       <c r="B17" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C17">
         <v>44</v>
       </c>
       <c r="D17" t="s">
-        <v>23</v>
-      </c>
-      <c r="E17" t="s">
-        <v>24</v>
+        <v>9</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -827,13 +838,13 @@
         <v>5</v>
       </c>
       <c r="B18" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C18">
         <v>44</v>
       </c>
       <c r="D18" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="E18" t="s">
         <v>24</v>
@@ -850,10 +861,7 @@
         <v>44</v>
       </c>
       <c r="D19" t="s">
-        <v>23</v>
-      </c>
-      <c r="E19" t="s">
-        <v>24</v>
+        <v>9</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -867,7 +875,7 @@
         <v>44</v>
       </c>
       <c r="D20" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="E20" t="s">
         <v>24</v>
@@ -878,16 +886,13 @@
         <v>5</v>
       </c>
       <c r="B21" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C21">
         <v>44</v>
       </c>
       <c r="D21" t="s">
-        <v>23</v>
-      </c>
-      <c r="E21" t="s">
-        <v>24</v>
+        <v>9</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -895,13 +900,13 @@
         <v>5</v>
       </c>
       <c r="B22" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C22">
         <v>44</v>
       </c>
       <c r="D22" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="E22" t="s">
         <v>24</v>
@@ -912,16 +917,13 @@
         <v>5</v>
       </c>
       <c r="B23" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C23">
         <v>44</v>
       </c>
       <c r="D23" t="s">
-        <v>23</v>
-      </c>
-      <c r="E23" t="s">
-        <v>24</v>
+        <v>9</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -929,16 +931,16 @@
         <v>5</v>
       </c>
       <c r="B24" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C24">
         <v>44</v>
       </c>
       <c r="D24" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="E24" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
     </row>
     <row r="25" spans="1:5">
@@ -946,16 +948,13 @@
         <v>5</v>
       </c>
       <c r="B25" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C25">
         <v>44</v>
       </c>
       <c r="D25" t="s">
-        <v>23</v>
-      </c>
-      <c r="E25" t="s">
-        <v>24</v>
+        <v>9</v>
       </c>
     </row>
     <row r="26" spans="1:5">
@@ -963,16 +962,16 @@
         <v>5</v>
       </c>
       <c r="B26" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C26">
         <v>44</v>
       </c>
       <c r="D26" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="E26" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
     </row>
     <row r="27" spans="1:5">
@@ -980,16 +979,603 @@
         <v>5</v>
       </c>
       <c r="B27" t="s">
+        <v>34</v>
+      </c>
+      <c r="C27">
+        <v>44</v>
+      </c>
+      <c r="D27" t="s">
+        <v>11</v>
+      </c>
+      <c r="E27" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28" t="s">
+        <v>5</v>
+      </c>
+      <c r="B28" t="s">
         <v>36</v>
       </c>
-      <c r="C27">
-        <v>44</v>
-      </c>
-      <c r="D27" t="s">
-        <v>23</v>
-      </c>
-      <c r="E27" t="s">
-        <v>24</v>
+      <c r="C28">
+        <v>44</v>
+      </c>
+      <c r="D28" t="s">
+        <v>11</v>
+      </c>
+      <c r="E28" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29" t="s">
+        <v>5</v>
+      </c>
+      <c r="B29" t="s">
+        <v>38</v>
+      </c>
+      <c r="C29">
+        <v>44</v>
+      </c>
+      <c r="D29" t="s">
+        <v>11</v>
+      </c>
+      <c r="E29" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30" t="s">
+        <v>5</v>
+      </c>
+      <c r="B30" t="s">
+        <v>38</v>
+      </c>
+      <c r="C30">
+        <v>44</v>
+      </c>
+      <c r="D30" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31" t="s">
+        <v>5</v>
+      </c>
+      <c r="B31" t="s">
+        <v>39</v>
+      </c>
+      <c r="C31">
+        <v>44</v>
+      </c>
+      <c r="D31" t="s">
+        <v>11</v>
+      </c>
+      <c r="E31" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32" t="s">
+        <v>5</v>
+      </c>
+      <c r="B32" t="s">
+        <v>39</v>
+      </c>
+      <c r="C32">
+        <v>44</v>
+      </c>
+      <c r="D32" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="A33" t="s">
+        <v>5</v>
+      </c>
+      <c r="B33" t="s">
+        <v>40</v>
+      </c>
+      <c r="C33">
+        <v>44</v>
+      </c>
+      <c r="D33" t="s">
+        <v>11</v>
+      </c>
+      <c r="E33" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="A34" t="s">
+        <v>5</v>
+      </c>
+      <c r="B34" t="s">
+        <v>41</v>
+      </c>
+      <c r="C34">
+        <v>44</v>
+      </c>
+      <c r="D34" t="s">
+        <v>11</v>
+      </c>
+      <c r="E34" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5">
+      <c r="A35" t="s">
+        <v>5</v>
+      </c>
+      <c r="B35" t="s">
+        <v>42</v>
+      </c>
+      <c r="C35">
+        <v>44</v>
+      </c>
+      <c r="D35" t="s">
+        <v>11</v>
+      </c>
+      <c r="E35" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
+      <c r="A36" t="s">
+        <v>5</v>
+      </c>
+      <c r="B36" t="s">
+        <v>42</v>
+      </c>
+      <c r="C36">
+        <v>44</v>
+      </c>
+      <c r="D36" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5">
+      <c r="A37" t="s">
+        <v>5</v>
+      </c>
+      <c r="B37" t="s">
+        <v>44</v>
+      </c>
+      <c r="C37">
+        <v>44</v>
+      </c>
+      <c r="D37" t="s">
+        <v>11</v>
+      </c>
+      <c r="E37" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5">
+      <c r="A38" t="s">
+        <v>5</v>
+      </c>
+      <c r="B38" t="s">
+        <v>45</v>
+      </c>
+      <c r="C38">
+        <v>44</v>
+      </c>
+      <c r="D38" t="s">
+        <v>11</v>
+      </c>
+      <c r="E38" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5">
+      <c r="A39" t="s">
+        <v>5</v>
+      </c>
+      <c r="B39" t="s">
+        <v>45</v>
+      </c>
+      <c r="C39">
+        <v>44</v>
+      </c>
+      <c r="D39" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5">
+      <c r="A40" t="s">
+        <v>5</v>
+      </c>
+      <c r="B40" t="s">
+        <v>46</v>
+      </c>
+      <c r="C40">
+        <v>44</v>
+      </c>
+      <c r="D40" t="s">
+        <v>11</v>
+      </c>
+      <c r="E40" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5">
+      <c r="A41" t="s">
+        <v>5</v>
+      </c>
+      <c r="B41" t="s">
+        <v>46</v>
+      </c>
+      <c r="C41">
+        <v>44</v>
+      </c>
+      <c r="D41" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5">
+      <c r="A42" t="s">
+        <v>5</v>
+      </c>
+      <c r="B42" t="s">
+        <v>48</v>
+      </c>
+      <c r="C42">
+        <v>44</v>
+      </c>
+      <c r="D42" t="s">
+        <v>11</v>
+      </c>
+      <c r="E42" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5">
+      <c r="A43" t="s">
+        <v>5</v>
+      </c>
+      <c r="B43" t="s">
+        <v>48</v>
+      </c>
+      <c r="C43">
+        <v>44</v>
+      </c>
+      <c r="D43" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5">
+      <c r="A44" t="s">
+        <v>5</v>
+      </c>
+      <c r="B44" t="s">
+        <v>49</v>
+      </c>
+      <c r="C44">
+        <v>44</v>
+      </c>
+      <c r="D44" t="s">
+        <v>11</v>
+      </c>
+      <c r="E44" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5">
+      <c r="A45" t="s">
+        <v>5</v>
+      </c>
+      <c r="B45" t="s">
+        <v>49</v>
+      </c>
+      <c r="C45">
+        <v>44</v>
+      </c>
+      <c r="D45" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5">
+      <c r="A46" t="s">
+        <v>5</v>
+      </c>
+      <c r="B46" t="s">
+        <v>50</v>
+      </c>
+      <c r="C46">
+        <v>44</v>
+      </c>
+      <c r="D46" t="s">
+        <v>11</v>
+      </c>
+      <c r="E46" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5">
+      <c r="A47" t="s">
+        <v>5</v>
+      </c>
+      <c r="B47" t="s">
+        <v>50</v>
+      </c>
+      <c r="C47">
+        <v>44</v>
+      </c>
+      <c r="D47" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5">
+      <c r="A48" t="s">
+        <v>5</v>
+      </c>
+      <c r="B48" t="s">
+        <v>51</v>
+      </c>
+      <c r="C48">
+        <v>44</v>
+      </c>
+      <c r="D48" t="s">
+        <v>11</v>
+      </c>
+      <c r="E48" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5">
+      <c r="A49" t="s">
+        <v>5</v>
+      </c>
+      <c r="B49" t="s">
+        <v>52</v>
+      </c>
+      <c r="C49">
+        <v>44</v>
+      </c>
+      <c r="D49" t="s">
+        <v>11</v>
+      </c>
+      <c r="E49" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5">
+      <c r="A50" t="s">
+        <v>5</v>
+      </c>
+      <c r="B50" t="s">
+        <v>52</v>
+      </c>
+      <c r="C50">
+        <v>44</v>
+      </c>
+      <c r="D50" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5">
+      <c r="A51" t="s">
+        <v>5</v>
+      </c>
+      <c r="B51" t="s">
+        <v>53</v>
+      </c>
+      <c r="C51">
+        <v>44</v>
+      </c>
+      <c r="D51" t="s">
+        <v>11</v>
+      </c>
+      <c r="E51" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5">
+      <c r="A52" t="s">
+        <v>5</v>
+      </c>
+      <c r="B52" t="s">
+        <v>54</v>
+      </c>
+      <c r="C52">
+        <v>44</v>
+      </c>
+      <c r="D52" t="s">
+        <v>11</v>
+      </c>
+      <c r="E52" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5">
+      <c r="A53" t="s">
+        <v>5</v>
+      </c>
+      <c r="B53" t="s">
+        <v>54</v>
+      </c>
+      <c r="C53">
+        <v>44</v>
+      </c>
+      <c r="D53" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5">
+      <c r="A54" t="s">
+        <v>5</v>
+      </c>
+      <c r="B54" t="s">
+        <v>55</v>
+      </c>
+      <c r="C54">
+        <v>44</v>
+      </c>
+      <c r="D54" t="s">
+        <v>11</v>
+      </c>
+      <c r="E54" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5">
+      <c r="A55" t="s">
+        <v>5</v>
+      </c>
+      <c r="B55" t="s">
+        <v>56</v>
+      </c>
+      <c r="C55">
+        <v>44</v>
+      </c>
+      <c r="D55" t="s">
+        <v>11</v>
+      </c>
+      <c r="E55" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5">
+      <c r="A56" t="s">
+        <v>5</v>
+      </c>
+      <c r="B56" t="s">
+        <v>56</v>
+      </c>
+      <c r="C56">
+        <v>44</v>
+      </c>
+      <c r="D56" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5">
+      <c r="A57" t="s">
+        <v>5</v>
+      </c>
+      <c r="B57" t="s">
+        <v>57</v>
+      </c>
+      <c r="C57">
+        <v>44</v>
+      </c>
+      <c r="D57" t="s">
+        <v>11</v>
+      </c>
+      <c r="E57" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5">
+      <c r="A58" t="s">
+        <v>5</v>
+      </c>
+      <c r="B58" t="s">
+        <v>58</v>
+      </c>
+      <c r="C58">
+        <v>44</v>
+      </c>
+      <c r="D58" t="s">
+        <v>11</v>
+      </c>
+      <c r="E58" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5">
+      <c r="A59" t="s">
+        <v>5</v>
+      </c>
+      <c r="B59" t="s">
+        <v>58</v>
+      </c>
+      <c r="C59">
+        <v>44</v>
+      </c>
+      <c r="D59" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5">
+      <c r="A60" t="s">
+        <v>5</v>
+      </c>
+      <c r="B60" t="s">
+        <v>59</v>
+      </c>
+      <c r="C60">
+        <v>44</v>
+      </c>
+      <c r="D60" t="s">
+        <v>11</v>
+      </c>
+      <c r="E60" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5">
+      <c r="A61" t="s">
+        <v>5</v>
+      </c>
+      <c r="B61" t="s">
+        <v>59</v>
+      </c>
+      <c r="C61">
+        <v>44</v>
+      </c>
+      <c r="D61" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5">
+      <c r="A62" t="s">
+        <v>5</v>
+      </c>
+      <c r="B62" t="s">
+        <v>61</v>
+      </c>
+      <c r="C62">
+        <v>44</v>
+      </c>
+      <c r="D62" t="s">
+        <v>11</v>
+      </c>
+      <c r="E62" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5">
+      <c r="A63" t="s">
+        <v>5</v>
+      </c>
+      <c r="B63" t="s">
+        <v>61</v>
+      </c>
+      <c r="C63">
+        <v>44</v>
+      </c>
+      <c r="D63" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5">
+      <c r="A64" t="s">
+        <v>5</v>
+      </c>
+      <c r="B64" t="s">
+        <v>62</v>
+      </c>
+      <c r="C64">
+        <v>44</v>
+      </c>
+      <c r="D64" t="s">
+        <v>11</v>
+      </c>
+      <c r="E64" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>